<commit_message>
worked on method to merge notes from old report
</commit_message>
<xml_diff>
--- a/reports_project/new_month_report/new_report_1.xlsx
+++ b/reports_project/new_month_report/new_report_1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF6B77C-1168-CC4E-B5DE-421E1CA6471C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF35F9F8-A3D1-024D-86FB-CC41E43D0599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5260" yWindow="3400" windowWidth="23440" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,7 +630,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -699,20 +699,11 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -742,7 +733,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -750,7 +740,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color rgb="FFE2E2E2"/>
         </left>
@@ -780,6 +770,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -787,7 +778,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FFE2E2E2"/>
         </left>
@@ -2574,8 +2565,8 @@
     <tableColumn id="6" xr3:uid="{2488AE99-3DE2-4129-BFDC-71F8F04611E1}" name="Title" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{A0E81232-02AE-4C14-A66E-69BC3FEA4A55}" name="WGI DATE" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{76F0FE5A-05C3-4285-8669-6D894F30E42E}" name="SCD WGI YMD" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{ECB1F6C5-1706-4772-8D39-14796F7D5F2A}" name="Organization Cd" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{B659E2C5-C0C3-40FD-8535-373A47309D11}" name="Longtitle" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{ECB1F6C5-1706-4772-8D39-14796F7D5F2A}" name="Organization Cd" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{B659E2C5-C0C3-40FD-8535-373A47309D11}" name="Longtitle" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5397,7 +5388,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A2:A15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5506,19 +5497,19 @@
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="22">
         <v>45292</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
       <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5528,19 +5519,19 @@
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="22">
         <v>45296</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
       <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5550,19 +5541,19 @@
       <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="22">
         <v>45330</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
       <c r="N6" s="16"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5572,19 +5563,19 @@
       <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="22">
         <v>45339</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
       <c r="N7" s="16"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5594,19 +5585,19 @@
       <c r="B8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="22">
         <v>45347</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="16"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5616,19 +5607,19 @@
       <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="22">
         <v>45349</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -5637,19 +5628,19 @@
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="22">
         <v>45308</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5658,19 +5649,19 @@
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="22">
         <v>45318</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -5679,19 +5670,19 @@
       <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="22">
         <v>45601</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -5700,19 +5691,19 @@
       <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="22">
         <v>45318</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -5721,19 +5712,19 @@
       <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="22">
         <v>45394</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -5742,19 +5733,19 @@
       <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="22">
         <v>45512</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -5763,19 +5754,19 @@
       <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="22">
         <v>45488</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -5784,19 +5775,19 @@
       <c r="B17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="22">
         <v>45489</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -5805,19 +5796,19 @@
       <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="22">
         <v>45397</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -5826,19 +5817,19 @@
       <c r="B19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="22">
         <v>45461</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -5847,19 +5838,19 @@
       <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="22">
         <v>45448</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -5868,19 +5859,19 @@
       <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="22">
         <v>45450</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -5889,19 +5880,19 @@
       <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="22">
         <v>45323</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -5910,19 +5901,19 @@
       <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="22">
         <v>45570</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -5931,19 +5922,19 @@
       <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="22">
         <v>45536</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5958,8 +5949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300C2578-2525-4DC1-B795-16107A4AB6FC}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6022,7 +6013,7 @@
         <v>45935</v>
       </c>
       <c r="H2" s="20"/>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="28" t="s">
         <v>134</v>
       </c>
       <c r="J2" s="19"/>
@@ -6040,7 +6031,7 @@
         <v>45949</v>
       </c>
       <c r="H3" s="20"/>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="28" t="s">
         <v>39</v>
       </c>
       <c r="J3" s="19"/>
@@ -6058,7 +6049,7 @@
         <v>45949</v>
       </c>
       <c r="H4" s="20"/>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="28" t="s">
         <v>38</v>
       </c>
       <c r="J4" s="19"/>
@@ -6076,7 +6067,7 @@
         <v>45949</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="28" t="s">
         <v>135</v>
       </c>
       <c r="J5" s="19"/>
@@ -6094,7 +6085,7 @@
         <v>45963</v>
       </c>
       <c r="H6" s="20"/>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="28" t="s">
         <v>136</v>
       </c>
       <c r="J6" s="19"/>
@@ -6112,7 +6103,7 @@
         <v>45963</v>
       </c>
       <c r="H7" s="20"/>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="28" t="s">
         <v>137</v>
       </c>
       <c r="J7" s="19"/>
@@ -6130,7 +6121,7 @@
         <v>45977</v>
       </c>
       <c r="H8" s="20"/>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="28" t="s">
         <v>134</v>
       </c>
       <c r="J8" s="19"/>
@@ -6148,7 +6139,7 @@
         <v>45991</v>
       </c>
       <c r="H9" s="20"/>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="28" t="s">
         <v>39</v>
       </c>
       <c r="J9" s="19"/>
@@ -6166,7 +6157,7 @@
         <v>45991</v>
       </c>
       <c r="H10" s="20"/>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="28" t="s">
         <v>38</v>
       </c>
       <c r="J10" s="19"/>
@@ -6184,7 +6175,7 @@
         <v>46019</v>
       </c>
       <c r="H11" s="20"/>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="28" t="s">
         <v>135</v>
       </c>
       <c r="J11" s="19"/>
@@ -6202,7 +6193,7 @@
         <v>46019</v>
       </c>
       <c r="H12" s="20"/>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="28" t="s">
         <v>136</v>
       </c>
       <c r="J12" s="19"/>
@@ -6220,7 +6211,7 @@
         <v>46033</v>
       </c>
       <c r="H13" s="20"/>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="28" t="s">
         <v>137</v>
       </c>
       <c r="J13" s="19"/>
@@ -6238,7 +6229,7 @@
         <v>46033</v>
       </c>
       <c r="H14" s="20"/>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="28" t="s">
         <v>134</v>
       </c>
       <c r="J14" s="19"/>
@@ -6256,7 +6247,7 @@
         <v>46047</v>
       </c>
       <c r="H15" s="20"/>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="28" t="s">
         <v>39</v>
       </c>
       <c r="J15" s="19"/>
@@ -6271,16 +6262,53 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocIdPersistId xmlns="bf465682-a195-48e8-a373-685144231e9c">true</_dlc_DocIdPersistId>
-    <_dlc_DocId xmlns="bf465682-a195-48e8-a373-685144231e9c">WCVJDXXHMT7D-945044613-85</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="bf465682-a195-48e8-a373-685144231e9c">
-      <Url>https://cisgov.sharepoint.com/sites/ECNhct/Offices/hct/HRIT/HCTReportingCenter/_layouts/15/DocIdRedir.aspx?ID=WCVJDXXHMT7D-945044613-85</Url>
-      <Description>WCVJDXXHMT7D-945044613-85</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6458,53 +6486,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocIdPersistId xmlns="bf465682-a195-48e8-a373-685144231e9c">true</_dlc_DocIdPersistId>
+    <_dlc_DocId xmlns="bf465682-a195-48e8-a373-685144231e9c">WCVJDXXHMT7D-945044613-85</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="bf465682-a195-48e8-a373-685144231e9c">
+      <Url>https://cisgov.sharepoint.com/sites/ECNhct/Offices/hct/HRIT/HCTReportingCenter/_layouts/15/DocIdRedir.aspx?ID=WCVJDXXHMT7D-945044613-85</Url>
+      <Description>WCVJDXXHMT7D-945044613-85</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6513,18 +6504,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DE39C24-384E-4C44-9878-44FE0A7BA72C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D16E658-4C8F-4C0E-B7D2-CFF9B31601AF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c5ed04f4-622d-4734-9b15-89f52925a551"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bf465682-a195-48e8-a373-685144231e9c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6549,9 +6531,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D16E658-4C8F-4C0E-B7D2-CFF9B31601AF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DE39C24-384E-4C44-9878-44FE0A7BA72C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c5ed04f4-622d-4734-9b15-89f52925a551"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bf465682-a195-48e8-a373-685144231e9c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
worked on method to bring in old month report
</commit_message>
<xml_diff>
--- a/reports_project/new_month_report/new_report_1.xlsx
+++ b/reports_project/new_month_report/new_report_1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10118"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF35F9F8-A3D1-024D-86FB-CC41E43D0599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790ADBAE-4645-504B-B751-AD79BCD15B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5260" yWindow="3400" windowWidth="23440" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,6 +716,1293 @@
     <cellStyle name="Normal 6" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="51">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF959595"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF959595"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF959595"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF959595"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF959595"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1155,1293 +2442,6 @@
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF959595"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF959595"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF959595"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF959595"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF959595"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2456,7 +2456,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C402898B-1F29-46AE-93E4-650D764269AA}" name="Table1" displayName="Table1" ref="A1:S91" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C402898B-1F29-46AE-93E4-650D764269AA}" name="Table1" displayName="Table1" ref="A1:S91" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="A1:S91" xr:uid="{C402898B-1F29-46AE-93E4-650D764269AA}">
     <filterColumn colId="0">
       <filters>
@@ -2475,32 +2475,32 @@
     <sortCondition ref="L1:L2"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C7725C49-BB83-4C9A-A839-3E1F0BD0EF85}" name="ORG CODE" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{DC445E5B-AF04-4357-90A5-B715F53662C6}" name="EMPLOYEE NAME" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{A692BDD1-1073-4260-9F12-3FEFBF6ED388}" name="POSITION TITLE" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{41CA3841-2F3A-4FEC-B74E-1E78A00E4017}" name="IPN" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{BFADDF9E-59B8-44FD-9FFC-B12C8BDA242B}" name="PP" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{9717FFE6-92CC-4025-815E-201C2BAA45D9}" name="SERIES" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{28DB058D-9AD7-4DD3-BE86-B1D35BC2F84A}" name="GD" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{37C78208-0B0D-4D36-82F0-50001A10716B}" name="TARGET GR" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{AF995B83-5E1F-40E5-ADC2-9C8039946EF7}" name="OFC" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{EC922F22-2B24-4572-BBC6-EA6A22EE1688}" name="CAT CODE" dataDxfId="38"/>
-    <tableColumn id="11" xr3:uid="{97CCC4C8-E7DA-44E2-A8CA-2AAEC1A7683A}" name="EOD CIS" dataDxfId="37"/>
-    <tableColumn id="12" xr3:uid="{E59B726E-A00A-4D3D-B1AF-72FE2492E707}" name="ENTER PRES GR" dataDxfId="36"/>
-    <tableColumn id="13" xr3:uid="{0832597D-76F3-4118-BE62-D2FF84094B99}" name="WORK SCHEDULE" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{0174AC6B-A3C0-478A-8680-C2D21A0FF39D}" name="ORG_CODE_LEVEL_2_DESCR" dataDxfId="34"/>
-    <tableColumn id="15" xr3:uid="{2C24532D-1A05-440D-8609-800F0E859016}" name="ORG_CODE_LEVEL_3_DESCR" dataDxfId="33"/>
-    <tableColumn id="16" xr3:uid="{3B601192-224A-4D72-AD2D-127E14CEED0E}" name="ORG_CODE_LEVEL_4_DESCR" dataDxfId="32"/>
-    <tableColumn id="17" xr3:uid="{B1085BB1-9551-48DC-8A9C-2452DB6CE6E3}" name="ORG_CODE_LEVEL_5_DESCR" dataDxfId="31"/>
-    <tableColumn id="18" xr3:uid="{80CC6877-F265-46D8-A06A-53E4836071C6}" name="CITY_NAME" dataDxfId="30"/>
-    <tableColumn id="19" xr3:uid="{D1F4502D-E328-45B2-A809-278CF0774A94}" name="STATE_NAME" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{C7725C49-BB83-4C9A-A839-3E1F0BD0EF85}" name="ORG CODE" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{DC445E5B-AF04-4357-90A5-B715F53662C6}" name="EMPLOYEE NAME" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{A692BDD1-1073-4260-9F12-3FEFBF6ED388}" name="POSITION TITLE" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{41CA3841-2F3A-4FEC-B74E-1E78A00E4017}" name="IPN" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{BFADDF9E-59B8-44FD-9FFC-B12C8BDA242B}" name="PP" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{9717FFE6-92CC-4025-815E-201C2BAA45D9}" name="SERIES" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{28DB058D-9AD7-4DD3-BE86-B1D35BC2F84A}" name="GD" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{37C78208-0B0D-4D36-82F0-50001A10716B}" name="TARGET GR" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{AF995B83-5E1F-40E5-ADC2-9C8039946EF7}" name="OFC" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{EC922F22-2B24-4572-BBC6-EA6A22EE1688}" name="CAT CODE" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{97CCC4C8-E7DA-44E2-A8CA-2AAEC1A7683A}" name="EOD CIS" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{E59B726E-A00A-4D3D-B1AF-72FE2492E707}" name="ENTER PRES GR" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{0832597D-76F3-4118-BE62-D2FF84094B99}" name="WORK SCHEDULE" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{0174AC6B-A3C0-478A-8680-C2D21A0FF39D}" name="ORG_CODE_LEVEL_2_DESCR" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{2C24532D-1A05-440D-8609-800F0E859016}" name="ORG_CODE_LEVEL_3_DESCR" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{3B601192-224A-4D72-AD2D-127E14CEED0E}" name="ORG_CODE_LEVEL_4_DESCR" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{B1085BB1-9551-48DC-8A9C-2452DB6CE6E3}" name="ORG_CODE_LEVEL_5_DESCR" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{80CC6877-F265-46D8-A06A-53E4836071C6}" name="CITY_NAME" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{D1F4502D-E328-45B2-A809-278CF0774A94}" name="STATE_NAME" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4AE4F922-F0EC-40B4-BC41-C699B2D6BAE4}" name="Table2" displayName="Table2" ref="A1:M24" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4AE4F922-F0EC-40B4-BC41-C699B2D6BAE4}" name="Table2" displayName="Table2" ref="A1:M24" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A1:M24" xr:uid="{4AE4F922-F0EC-40B4-BC41-C699B2D6BAE4}">
     <filterColumn colId="0">
       <filters>
@@ -2519,26 +2519,26 @@
     <sortCondition ref="C1:C3"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F9AF80B6-6878-4BA0-BAD5-DCEE169549F7}" name="ORG_CODE" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{3977BD6E-118A-4EE5-AF0A-553AA0A2C879}" name="Employee Name" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{9C44D2D0-F2B5-4B21-958A-2DB3CB909B06}" name="APPNT EFF DATE" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{3F8501AA-1D3B-4EB4-B17B-CDBE99D32D22}" name="APPNT NOA " dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{64104D61-D9FB-4D98-9B23-63AA56CB1EA9}" name="APPNT 1ST AUTH" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{C19C2C3E-F453-4BB2-ACEE-B991A9B4D2E0}" name="POSITION TITLE" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{C7B93B9A-AA5A-423F-8155-6B54CE1A003C}" name="SERIES" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{64745A3D-5027-4644-AF5E-62F2455DF9B7}" name="GRADE" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{8CB55901-EA7F-4349-A0AB-8E5891EEDC2A}" name="TENURE" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{FF0306F6-B6B4-43FF-B7BE-48CFADD0BF8A}" name="ORG_CODE_LEVEL_2_DESCR" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{BDB8FBA7-544F-41B8-AEED-9112DE31A7D5}" name="ORG_CODE_LEVEL_3_DESCR" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{989B987E-EC6A-460B-A0EC-D2F17CE3DAC8}" name="ORG_CODE_LEVEL_4_DESCR" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{679BC5AF-1890-4D76-AB72-DBF10D00E30B}" name="ORG_CODE_LEVEL_5_DESCR" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{F9AF80B6-6878-4BA0-BAD5-DCEE169549F7}" name="ORG_CODE" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{3977BD6E-118A-4EE5-AF0A-553AA0A2C879}" name="Employee Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{9C44D2D0-F2B5-4B21-958A-2DB3CB909B06}" name="APPNT EFF DATE" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{3F8501AA-1D3B-4EB4-B17B-CDBE99D32D22}" name="APPNT NOA " dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{64104D61-D9FB-4D98-9B23-63AA56CB1EA9}" name="APPNT 1ST AUTH" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{C19C2C3E-F453-4BB2-ACEE-B991A9B4D2E0}" name="POSITION TITLE" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{C7B93B9A-AA5A-423F-8155-6B54CE1A003C}" name="SERIES" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{64745A3D-5027-4644-AF5E-62F2455DF9B7}" name="GRADE" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{8CB55901-EA7F-4349-A0AB-8E5891EEDC2A}" name="TENURE" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{FF0306F6-B6B4-43FF-B7BE-48CFADD0BF8A}" name="ORG_CODE_LEVEL_2_DESCR" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{BDB8FBA7-544F-41B8-AEED-9112DE31A7D5}" name="ORG_CODE_LEVEL_3_DESCR" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{989B987E-EC6A-460B-A0EC-D2F17CE3DAC8}" name="ORG_CODE_LEVEL_4_DESCR" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{679BC5AF-1890-4D76-AB72-DBF10D00E30B}" name="ORG_CODE_LEVEL_5_DESCR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DC991E26-85FC-41E7-823E-BC2855330FD6}" name="Table4" displayName="Table4" ref="A1:J15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DC991E26-85FC-41E7-823E-BC2855330FD6}" name="Table4" displayName="Table4" ref="A1:J15" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="A1:J15" xr:uid="{DC991E26-85FC-41E7-823E-BC2855330FD6}">
     <filterColumn colId="8">
       <filters>
@@ -2557,16 +2557,16 @@
     <sortCondition ref="G1:G15"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{FA489DEB-2CC6-4FFB-B751-7C47891ABFFA}" name="Name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{9C50CAFC-6FEE-470B-A366-13333A2C73E5}" name="Pay Plan" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0E617942-B177-495B-88ED-60327A662577}" name="Grade" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{0A728D17-5C11-46D6-8C1E-DDDE33A91022}" name="Step" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{03792EBD-9895-4833-9BAA-FC0690C3A3D2}" name="Series" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{2488AE99-3DE2-4129-BFDC-71F8F04611E1}" name="Title" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{A0E81232-02AE-4C14-A66E-69BC3FEA4A55}" name="WGI DATE" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{76F0FE5A-05C3-4285-8669-6D894F30E42E}" name="SCD WGI YMD" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{ECB1F6C5-1706-4772-8D39-14796F7D5F2A}" name="Organization Cd" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{B659E2C5-C0C3-40FD-8535-373A47309D11}" name="Longtitle" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FA489DEB-2CC6-4FFB-B751-7C47891ABFFA}" name="Name" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{9C50CAFC-6FEE-470B-A366-13333A2C73E5}" name="Pay Plan" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{0E617942-B177-495B-88ED-60327A662577}" name="Grade" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{0A728D17-5C11-46D6-8C1E-DDDE33A91022}" name="Step" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{03792EBD-9895-4833-9BAA-FC0690C3A3D2}" name="Series" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{2488AE99-3DE2-4129-BFDC-71F8F04611E1}" name="Title" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{A0E81232-02AE-4C14-A66E-69BC3FEA4A55}" name="WGI DATE" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{76F0FE5A-05C3-4285-8669-6D894F30E42E}" name="SCD WGI YMD" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{ECB1F6C5-1706-4772-8D39-14796F7D5F2A}" name="Organization Cd" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{B659E2C5-C0C3-40FD-8535-373A47309D11}" name="Longtitle" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5950,7 +5950,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6312,6 +6312,24 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocIdPersistId xmlns="bf465682-a195-48e8-a373-685144231e9c">true</_dlc_DocIdPersistId>
+    <_dlc_DocId xmlns="bf465682-a195-48e8-a373-685144231e9c">WCVJDXXHMT7D-945044613-85</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="bf465682-a195-48e8-a373-685144231e9c">
+      <Url>https://cisgov.sharepoint.com/sites/ECNhct/Offices/hct/HRIT/HCTReportingCenter/_layouts/15/DocIdRedir.aspx?ID=WCVJDXXHMT7D-945044613-85</Url>
+      <Description>WCVJDXXHMT7D-945044613-85</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005AD585D709FE2F4E8E78CCAD878BB7B2" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86a8288cca08b2275286a7cc5415fffa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5ed04f4-622d-4734-9b15-89f52925a551" xmlns:ns3="bf465682-a195-48e8-a373-685144231e9c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ae85b8bc60391f2b6a9cfc680ba816" ns2:_="" ns3:_="">
     <xsd:import namespace="c5ed04f4-622d-4734-9b15-89f52925a551"/>
@@ -6485,24 +6503,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocIdPersistId xmlns="bf465682-a195-48e8-a373-685144231e9c">true</_dlc_DocIdPersistId>
-    <_dlc_DocId xmlns="bf465682-a195-48e8-a373-685144231e9c">WCVJDXXHMT7D-945044613-85</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="bf465682-a195-48e8-a373-685144231e9c">
-      <Url>https://cisgov.sharepoint.com/sites/ECNhct/Offices/hct/HRIT/HCTReportingCenter/_layouts/15/DocIdRedir.aspx?ID=WCVJDXXHMT7D-945044613-85</Url>
-      <Description>WCVJDXXHMT7D-945044613-85</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D16E658-4C8F-4C0E-B7D2-CFF9B31601AF}">
   <ds:schemaRefs>
@@ -6512,20 +6512,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38192834-6563-4BBD-B913-E3DA672C0E51}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73725FF9-00B7-448B-90C2-99B21669C715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c5ed04f4-622d-4734-9b15-89f52925a551"/>
-    <ds:schemaRef ds:uri="bf465682-a195-48e8-a373-685144231e9c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6548,9 +6537,20 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73725FF9-00B7-448B-90C2-99B21669C715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38192834-6563-4BBD-B913-E3DA672C0E51}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c5ed04f4-622d-4734-9b15-89f52925a551"/>
+    <ds:schemaRef ds:uri="bf465682-a195-48e8-a373-685144231e9c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>